<commit_message>
all done. i hope
</commit_message>
<xml_diff>
--- a/dsa_py/SortingAnalysis.xlsx
+++ b/dsa_py/SortingAnalysis.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D301"/>
+  <dimension ref="A1:E301"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,6 +439,11 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>Comparisons</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>Comparisions</t>
         </is>
       </c>
@@ -453,11 +458,12 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D2" t="n">
         <v>45</v>
       </c>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -469,9 +475,10 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>6</v>
-      </c>
-      <c r="D3" t="n">
+        <v>8</v>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="n">
         <v>45</v>
       </c>
     </row>
@@ -485,10 +492,11 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>14</v>
-      </c>
-      <c r="D4" t="n">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="5">
@@ -501,11 +509,12 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>75</v>
+        <v>85</v>
       </c>
       <c r="D5" t="n">
         <v>190</v>
       </c>
+      <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -517,9 +526,10 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>13</v>
-      </c>
-      <c r="D6" t="n">
+        <v>17</v>
+      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="n">
         <v>190</v>
       </c>
     </row>
@@ -533,10 +543,11 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>75</v>
-      </c>
-      <c r="D7" t="n">
-        <v>92</v>
+        <v>85</v>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>99</v>
       </c>
     </row>
     <row r="8">
@@ -549,11 +560,12 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>226</v>
+        <v>255</v>
       </c>
       <c r="D8" t="n">
         <v>435</v>
       </c>
+      <c r="E8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -565,9 +577,10 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>28</v>
-      </c>
-      <c r="D9" t="n">
+        <v>27</v>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="n">
         <v>435</v>
       </c>
     </row>
@@ -581,10 +594,11 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>226</v>
-      </c>
-      <c r="D10" t="n">
-        <v>247</v>
+        <v>255</v>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="n">
+        <v>281</v>
       </c>
     </row>
     <row r="11">
@@ -597,11 +611,12 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>359</v>
+        <v>384</v>
       </c>
       <c r="D11" t="n">
         <v>780</v>
       </c>
+      <c r="E11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -613,9 +628,10 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>33</v>
-      </c>
-      <c r="D12" t="n">
+        <v>36</v>
+      </c>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="n">
         <v>780</v>
       </c>
     </row>
@@ -629,10 +645,11 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>359</v>
-      </c>
-      <c r="D13" t="n">
-        <v>396</v>
+        <v>384</v>
+      </c>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="n">
+        <v>420</v>
       </c>
     </row>
     <row r="14">
@@ -645,11 +662,12 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>591</v>
+        <v>507</v>
       </c>
       <c r="D14" t="n">
         <v>1225</v>
       </c>
+      <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -661,9 +679,10 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>45</v>
-      </c>
-      <c r="D15" t="n">
+        <v>47</v>
+      </c>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="n">
         <v>1225</v>
       </c>
     </row>
@@ -677,10 +696,11 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>591</v>
-      </c>
-      <c r="D16" t="n">
-        <v>637</v>
+        <v>507</v>
+      </c>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="n">
+        <v>553</v>
       </c>
     </row>
     <row r="17">
@@ -693,11 +713,12 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>920</v>
+        <v>837</v>
       </c>
       <c r="D17" t="n">
         <v>1770</v>
       </c>
+      <c r="E17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -709,9 +730,10 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>54</v>
-      </c>
-      <c r="D18" t="n">
+        <v>57</v>
+      </c>
+      <c r="D18" t="inlineStr"/>
+      <c r="E18" t="n">
         <v>1770</v>
       </c>
     </row>
@@ -725,10 +747,11 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>920</v>
-      </c>
-      <c r="D19" t="n">
-        <v>975</v>
+        <v>837</v>
+      </c>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="n">
+        <v>889</v>
       </c>
     </row>
     <row r="20">
@@ -741,11 +764,12 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>1126</v>
+        <v>1171</v>
       </c>
       <c r="D20" t="n">
         <v>2415</v>
       </c>
+      <c r="E20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -757,9 +781,10 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>64</v>
-      </c>
-      <c r="D21" t="n">
+        <v>67</v>
+      </c>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="n">
         <v>2415</v>
       </c>
     </row>
@@ -773,10 +798,11 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1126</v>
-      </c>
-      <c r="D22" t="n">
-        <v>1193</v>
+        <v>1171</v>
+      </c>
+      <c r="D22" t="inlineStr"/>
+      <c r="E22" t="n">
+        <v>1235</v>
       </c>
     </row>
     <row r="23">
@@ -789,11 +815,12 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>1518</v>
+        <v>1521</v>
       </c>
       <c r="D23" t="n">
         <v>3160</v>
       </c>
+      <c r="E23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -805,9 +832,10 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>78</v>
-      </c>
-      <c r="D24" t="n">
+        <v>71</v>
+      </c>
+      <c r="D24" t="inlineStr"/>
+      <c r="E24" t="n">
         <v>3160</v>
       </c>
     </row>
@@ -821,10 +849,11 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1518</v>
-      </c>
-      <c r="D25" t="n">
-        <v>1594</v>
+        <v>1521</v>
+      </c>
+      <c r="D25" t="inlineStr"/>
+      <c r="E25" t="n">
+        <v>1600</v>
       </c>
     </row>
     <row r="26">
@@ -837,11 +866,12 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>2051</v>
+        <v>2060</v>
       </c>
       <c r="D26" t="n">
         <v>4005</v>
       </c>
+      <c r="E26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -853,9 +883,10 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>83</v>
-      </c>
-      <c r="D27" t="n">
+        <v>82</v>
+      </c>
+      <c r="D27" t="inlineStr"/>
+      <c r="E27" t="n">
         <v>4005</v>
       </c>
     </row>
@@ -869,10 +900,11 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>2051</v>
-      </c>
-      <c r="D28" t="n">
-        <v>2137</v>
+        <v>2060</v>
+      </c>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="n">
+        <v>2143</v>
       </c>
     </row>
     <row r="29">
@@ -885,11 +917,12 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>2624</v>
+        <v>2445</v>
       </c>
       <c r="D29" t="n">
         <v>4950</v>
       </c>
+      <c r="E29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -901,9 +934,10 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>90</v>
-      </c>
-      <c r="D30" t="n">
+        <v>93</v>
+      </c>
+      <c r="D30" t="inlineStr"/>
+      <c r="E30" t="n">
         <v>4950</v>
       </c>
     </row>
@@ -917,10 +951,11 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>2624</v>
-      </c>
-      <c r="D31" t="n">
-        <v>2718</v>
+        <v>2445</v>
+      </c>
+      <c r="D31" t="inlineStr"/>
+      <c r="E31" t="n">
+        <v>2540</v>
       </c>
     </row>
     <row r="32">
@@ -933,11 +968,12 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>2806</v>
+        <v>2793</v>
       </c>
       <c r="D32" t="n">
         <v>5995</v>
       </c>
+      <c r="E32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -949,9 +985,10 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>104</v>
-      </c>
-      <c r="D33" t="n">
+        <v>107</v>
+      </c>
+      <c r="D33" t="inlineStr"/>
+      <c r="E33" t="n">
         <v>5995</v>
       </c>
     </row>
@@ -965,10 +1002,11 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>2806</v>
-      </c>
-      <c r="D34" t="n">
-        <v>2909</v>
+        <v>2793</v>
+      </c>
+      <c r="D34" t="inlineStr"/>
+      <c r="E34" t="n">
+        <v>2899</v>
       </c>
     </row>
     <row r="35">
@@ -981,11 +1019,12 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>3721</v>
+        <v>3466</v>
       </c>
       <c r="D35" t="n">
         <v>7140</v>
       </c>
+      <c r="E35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -997,9 +1036,10 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>113</v>
-      </c>
-      <c r="D36" t="n">
+        <v>112</v>
+      </c>
+      <c r="D36" t="inlineStr"/>
+      <c r="E36" t="n">
         <v>7140</v>
       </c>
     </row>
@@ -1013,10 +1053,11 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>3721</v>
-      </c>
-      <c r="D37" t="n">
-        <v>3832</v>
+        <v>3466</v>
+      </c>
+      <c r="D37" t="inlineStr"/>
+      <c r="E37" t="n">
+        <v>3581</v>
       </c>
     </row>
     <row r="38">
@@ -1029,11 +1070,12 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>4439</v>
+        <v>4295</v>
       </c>
       <c r="D38" t="n">
         <v>8385</v>
       </c>
+      <c r="E38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -1045,9 +1087,10 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>123</v>
-      </c>
-      <c r="D39" t="n">
+        <v>124</v>
+      </c>
+      <c r="D39" t="inlineStr"/>
+      <c r="E39" t="n">
         <v>8385</v>
       </c>
     </row>
@@ -1061,10 +1104,11 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>4439</v>
-      </c>
-      <c r="D40" t="n">
-        <v>4562</v>
+        <v>4295</v>
+      </c>
+      <c r="D40" t="inlineStr"/>
+      <c r="E40" t="n">
+        <v>4420</v>
       </c>
     </row>
     <row r="41">
@@ -1077,11 +1121,12 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>5206</v>
+        <v>4873</v>
       </c>
       <c r="D41" t="n">
         <v>9730</v>
       </c>
+      <c r="E41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -1093,9 +1138,10 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>134</v>
-      </c>
-      <c r="D42" t="n">
+        <v>135</v>
+      </c>
+      <c r="D42" t="inlineStr"/>
+      <c r="E42" t="n">
         <v>9730</v>
       </c>
     </row>
@@ -1109,10 +1155,11 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>5206</v>
-      </c>
-      <c r="D43" t="n">
-        <v>5338</v>
+        <v>4873</v>
+      </c>
+      <c r="D43" t="inlineStr"/>
+      <c r="E43" t="n">
+        <v>5005</v>
       </c>
     </row>
     <row r="44">
@@ -1125,11 +1172,12 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>5696</v>
+        <v>6299</v>
       </c>
       <c r="D44" t="n">
         <v>11175</v>
       </c>
+      <c r="E44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -1141,9 +1189,10 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>146</v>
-      </c>
-      <c r="D45" t="n">
+        <v>145</v>
+      </c>
+      <c r="D45" t="inlineStr"/>
+      <c r="E45" t="n">
         <v>11175</v>
       </c>
     </row>
@@ -1157,10 +1206,11 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>5696</v>
-      </c>
-      <c r="D46" t="n">
-        <v>5841</v>
+        <v>6299</v>
+      </c>
+      <c r="D46" t="inlineStr"/>
+      <c r="E46" t="n">
+        <v>6441</v>
       </c>
     </row>
     <row r="47">
@@ -1173,11 +1223,12 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>6345</v>
+        <v>6554</v>
       </c>
       <c r="D47" t="n">
         <v>12720</v>
       </c>
+      <c r="E47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -1189,9 +1240,10 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>157</v>
-      </c>
-      <c r="D48" t="n">
+        <v>152</v>
+      </c>
+      <c r="D48" t="inlineStr"/>
+      <c r="E48" t="n">
         <v>12720</v>
       </c>
     </row>
@@ -1205,10 +1257,11 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>6345</v>
-      </c>
-      <c r="D49" t="n">
-        <v>6497</v>
+        <v>6554</v>
+      </c>
+      <c r="D49" t="inlineStr"/>
+      <c r="E49" t="n">
+        <v>6708</v>
       </c>
     </row>
     <row r="50">
@@ -1221,11 +1274,12 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>7429</v>
+        <v>7693</v>
       </c>
       <c r="D50" t="n">
         <v>14365</v>
       </c>
+      <c r="E50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -1237,9 +1291,10 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>161</v>
-      </c>
-      <c r="D51" t="n">
+        <v>163</v>
+      </c>
+      <c r="D51" t="inlineStr"/>
+      <c r="E51" t="n">
         <v>14365</v>
       </c>
     </row>
@@ -1253,10 +1308,11 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>7429</v>
-      </c>
-      <c r="D52" t="n">
-        <v>7593</v>
+        <v>7693</v>
+      </c>
+      <c r="D52" t="inlineStr"/>
+      <c r="E52" t="n">
+        <v>7859</v>
       </c>
     </row>
     <row r="53">
@@ -1269,11 +1325,12 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>8019</v>
+        <v>7623</v>
       </c>
       <c r="D53" t="n">
         <v>16110</v>
       </c>
+      <c r="E53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -1285,9 +1342,10 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>175</v>
-      </c>
-      <c r="D54" t="n">
+        <v>171</v>
+      </c>
+      <c r="D54" t="inlineStr"/>
+      <c r="E54" t="n">
         <v>16110</v>
       </c>
     </row>
@@ -1301,10 +1359,11 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>8019</v>
-      </c>
-      <c r="D55" t="n">
-        <v>8196</v>
+        <v>7623</v>
+      </c>
+      <c r="D55" t="inlineStr"/>
+      <c r="E55" t="n">
+        <v>7802</v>
       </c>
     </row>
     <row r="56">
@@ -1317,11 +1376,12 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>9284</v>
+        <v>8489</v>
       </c>
       <c r="D56" t="n">
         <v>17955</v>
       </c>
+      <c r="E56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -1333,9 +1393,10 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>186</v>
-      </c>
-      <c r="D57" t="n">
+        <v>177</v>
+      </c>
+      <c r="D57" t="inlineStr"/>
+      <c r="E57" t="n">
         <v>17955</v>
       </c>
     </row>
@@ -1349,10 +1410,11 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>9284</v>
-      </c>
-      <c r="D58" t="n">
-        <v>9468</v>
+        <v>8489</v>
+      </c>
+      <c r="D58" t="inlineStr"/>
+      <c r="E58" t="n">
+        <v>8674</v>
       </c>
     </row>
     <row r="59">
@@ -1365,11 +1427,12 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>10053</v>
+        <v>9628</v>
       </c>
       <c r="D59" t="n">
         <v>19900</v>
       </c>
+      <c r="E59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -1381,9 +1444,10 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>192</v>
-      </c>
-      <c r="D60" t="n">
+        <v>194</v>
+      </c>
+      <c r="D60" t="inlineStr"/>
+      <c r="E60" t="n">
         <v>19900</v>
       </c>
     </row>
@@ -1397,10 +1461,11 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>10053</v>
-      </c>
-      <c r="D61" t="n">
-        <v>10245</v>
+        <v>9628</v>
+      </c>
+      <c r="D61" t="inlineStr"/>
+      <c r="E61" t="n">
+        <v>9823</v>
       </c>
     </row>
     <row r="62">
@@ -1413,11 +1478,12 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>11592</v>
+        <v>10392</v>
       </c>
       <c r="D62" t="n">
         <v>21945</v>
       </c>
+      <c r="E62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -1429,9 +1495,10 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>205</v>
-      </c>
-      <c r="D63" t="n">
+        <v>207</v>
+      </c>
+      <c r="D63" t="inlineStr"/>
+      <c r="E63" t="n">
         <v>21945</v>
       </c>
     </row>
@@ -1445,10 +1512,11 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>11592</v>
-      </c>
-      <c r="D64" t="n">
-        <v>11798</v>
+        <v>10392</v>
+      </c>
+      <c r="D64" t="inlineStr"/>
+      <c r="E64" t="n">
+        <v>10597</v>
       </c>
     </row>
     <row r="65">
@@ -1461,11 +1529,12 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>11845</v>
+        <v>12788</v>
       </c>
       <c r="D65" t="n">
         <v>24090</v>
       </c>
+      <c r="E65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -1477,9 +1546,10 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>217</v>
-      </c>
-      <c r="D66" t="n">
+        <v>215</v>
+      </c>
+      <c r="D66" t="inlineStr"/>
+      <c r="E66" t="n">
         <v>24090</v>
       </c>
     </row>
@@ -1493,10 +1563,11 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>11845</v>
-      </c>
-      <c r="D67" t="n">
-        <v>12061</v>
+        <v>12788</v>
+      </c>
+      <c r="D67" t="inlineStr"/>
+      <c r="E67" t="n">
+        <v>12999</v>
       </c>
     </row>
     <row r="68">
@@ -1509,11 +1580,12 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>12946</v>
+        <v>12877</v>
       </c>
       <c r="D68" t="n">
         <v>26335</v>
       </c>
+      <c r="E68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -1525,9 +1597,10 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>227</v>
-      </c>
-      <c r="D69" t="n">
+        <v>224</v>
+      </c>
+      <c r="D69" t="inlineStr"/>
+      <c r="E69" t="n">
         <v>26335</v>
       </c>
     </row>
@@ -1541,10 +1614,11 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>12946</v>
-      </c>
-      <c r="D70" t="n">
-        <v>13173</v>
+        <v>12877</v>
+      </c>
+      <c r="D70" t="inlineStr"/>
+      <c r="E70" t="n">
+        <v>13102</v>
       </c>
     </row>
     <row r="71">
@@ -1557,11 +1631,12 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>14769</v>
+        <v>13186</v>
       </c>
       <c r="D71" t="n">
         <v>28680</v>
       </c>
+      <c r="E71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -1573,9 +1648,10 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>230</v>
-      </c>
-      <c r="D72" t="n">
+        <v>234</v>
+      </c>
+      <c r="D72" t="inlineStr"/>
+      <c r="E72" t="n">
         <v>28680</v>
       </c>
     </row>
@@ -1589,10 +1665,11 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>14769</v>
-      </c>
-      <c r="D73" t="n">
-        <v>15003</v>
+        <v>13186</v>
+      </c>
+      <c r="D73" t="inlineStr"/>
+      <c r="E73" t="n">
+        <v>13421</v>
       </c>
     </row>
     <row r="74">
@@ -1605,11 +1682,12 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>15886</v>
+        <v>15877</v>
       </c>
       <c r="D74" t="n">
         <v>31125</v>
       </c>
+      <c r="E74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -1623,7 +1701,8 @@
       <c r="C75" t="n">
         <v>243</v>
       </c>
-      <c r="D75" t="n">
+      <c r="D75" t="inlineStr"/>
+      <c r="E75" t="n">
         <v>31125</v>
       </c>
     </row>
@@ -1637,10 +1716,11 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>15886</v>
-      </c>
-      <c r="D76" t="n">
-        <v>16131</v>
+        <v>15877</v>
+      </c>
+      <c r="D76" t="inlineStr"/>
+      <c r="E76" t="n">
+        <v>16121</v>
       </c>
     </row>
     <row r="77">
@@ -1653,11 +1733,12 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>16191</v>
+        <v>16999</v>
       </c>
       <c r="D77" t="n">
         <v>33670</v>
       </c>
+      <c r="E77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -1669,9 +1750,10 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>252</v>
-      </c>
-      <c r="D78" t="n">
+        <v>256</v>
+      </c>
+      <c r="D78" t="inlineStr"/>
+      <c r="E78" t="n">
         <v>33670</v>
       </c>
     </row>
@@ -1685,10 +1767,11 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>16191</v>
-      </c>
-      <c r="D79" t="n">
-        <v>16443</v>
+        <v>16999</v>
+      </c>
+      <c r="D79" t="inlineStr"/>
+      <c r="E79" t="n">
+        <v>17250</v>
       </c>
     </row>
     <row r="80">
@@ -1701,11 +1784,12 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>19303</v>
+        <v>18024</v>
       </c>
       <c r="D80" t="n">
         <v>36315</v>
       </c>
+      <c r="E80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -1717,9 +1801,10 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>267</v>
-      </c>
-      <c r="D81" t="n">
+        <v>268</v>
+      </c>
+      <c r="D81" t="inlineStr"/>
+      <c r="E81" t="n">
         <v>36315</v>
       </c>
     </row>
@@ -1733,10 +1818,11 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>19303</v>
-      </c>
-      <c r="D82" t="n">
-        <v>19564</v>
+        <v>18024</v>
+      </c>
+      <c r="D82" t="inlineStr"/>
+      <c r="E82" t="n">
+        <v>18291</v>
       </c>
     </row>
     <row r="83">
@@ -1749,11 +1835,12 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>19393</v>
+        <v>20276</v>
       </c>
       <c r="D83" t="n">
         <v>39060</v>
       </c>
+      <c r="E83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -1765,9 +1852,10 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>275</v>
-      </c>
-      <c r="D84" t="n">
+        <v>271</v>
+      </c>
+      <c r="D84" t="inlineStr"/>
+      <c r="E84" t="n">
         <v>39060</v>
       </c>
     </row>
@@ -1781,10 +1869,11 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>19393</v>
-      </c>
-      <c r="D85" t="n">
-        <v>19668</v>
+        <v>20276</v>
+      </c>
+      <c r="D85" t="inlineStr"/>
+      <c r="E85" t="n">
+        <v>20546</v>
       </c>
     </row>
     <row r="86">
@@ -1797,11 +1886,12 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>21661</v>
+        <v>22262</v>
       </c>
       <c r="D86" t="n">
         <v>41905</v>
       </c>
+      <c r="E86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -1813,9 +1903,10 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>286</v>
-      </c>
-      <c r="D87" t="n">
+        <v>284</v>
+      </c>
+      <c r="D87" t="inlineStr"/>
+      <c r="E87" t="n">
         <v>41905</v>
       </c>
     </row>
@@ -1829,10 +1920,11 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>21661</v>
-      </c>
-      <c r="D88" t="n">
-        <v>21944</v>
+        <v>22262</v>
+      </c>
+      <c r="D88" t="inlineStr"/>
+      <c r="E88" t="n">
+        <v>22540</v>
       </c>
     </row>
     <row r="89">
@@ -1845,11 +1937,12 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>23234</v>
+        <v>22929</v>
       </c>
       <c r="D89" t="n">
         <v>44850</v>
       </c>
+      <c r="E89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -1863,7 +1956,8 @@
       <c r="C90" t="n">
         <v>293</v>
       </c>
-      <c r="D90" t="n">
+      <c r="D90" t="inlineStr"/>
+      <c r="E90" t="n">
         <v>44850</v>
       </c>
     </row>
@@ -1877,10 +1971,11 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>23234</v>
-      </c>
-      <c r="D91" t="n">
-        <v>23531</v>
+        <v>22929</v>
+      </c>
+      <c r="D91" t="inlineStr"/>
+      <c r="E91" t="n">
+        <v>23222</v>
       </c>
     </row>
     <row r="92">
@@ -1893,11 +1988,12 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>24090</v>
+        <v>24738</v>
       </c>
       <c r="D92" t="n">
         <v>47895</v>
       </c>
+      <c r="E92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="n">
@@ -1909,9 +2005,10 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>306</v>
-      </c>
-      <c r="D93" t="n">
+        <v>305</v>
+      </c>
+      <c r="D93" t="inlineStr"/>
+      <c r="E93" t="n">
         <v>47895</v>
       </c>
     </row>
@@ -1925,10 +2022,11 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>24090</v>
-      </c>
-      <c r="D94" t="n">
-        <v>24397</v>
+        <v>24738</v>
+      </c>
+      <c r="D94" t="inlineStr"/>
+      <c r="E94" t="n">
+        <v>25043</v>
       </c>
     </row>
     <row r="95">
@@ -1941,11 +2039,12 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>26494</v>
+        <v>26563</v>
       </c>
       <c r="D95" t="n">
         <v>51040</v>
       </c>
+      <c r="E95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -1957,9 +2056,10 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>313</v>
-      </c>
-      <c r="D96" t="n">
+        <v>314</v>
+      </c>
+      <c r="D96" t="inlineStr"/>
+      <c r="E96" t="n">
         <v>51040</v>
       </c>
     </row>
@@ -1973,10 +2073,11 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>26494</v>
-      </c>
-      <c r="D97" t="n">
-        <v>26808</v>
+        <v>26563</v>
+      </c>
+      <c r="D97" t="inlineStr"/>
+      <c r="E97" t="n">
+        <v>26877</v>
       </c>
     </row>
     <row r="98">
@@ -1989,11 +2090,12 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>25946</v>
+        <v>27900</v>
       </c>
       <c r="D98" t="n">
         <v>54285</v>
       </c>
+      <c r="E98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="n">
@@ -2005,9 +2107,10 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>323</v>
-      </c>
-      <c r="D99" t="n">
+        <v>322</v>
+      </c>
+      <c r="D99" t="inlineStr"/>
+      <c r="E99" t="n">
         <v>54285</v>
       </c>
     </row>
@@ -2021,10 +2124,11 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>25946</v>
-      </c>
-      <c r="D100" t="n">
-        <v>26271</v>
+        <v>27900</v>
+      </c>
+      <c r="D100" t="inlineStr"/>
+      <c r="E100" t="n">
+        <v>28222</v>
       </c>
     </row>
     <row r="101">
@@ -2037,11 +2141,12 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>26794</v>
+        <v>28055</v>
       </c>
       <c r="D101" t="n">
         <v>57630</v>
       </c>
+      <c r="E101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="n">
@@ -2053,9 +2158,10 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>336</v>
-      </c>
-      <c r="D102" t="n">
+        <v>333</v>
+      </c>
+      <c r="D102" t="inlineStr"/>
+      <c r="E102" t="n">
         <v>57630</v>
       </c>
     </row>
@@ -2069,10 +2175,11 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>26794</v>
-      </c>
-      <c r="D103" t="n">
-        <v>27128</v>
+        <v>28055</v>
+      </c>
+      <c r="D103" t="inlineStr"/>
+      <c r="E103" t="n">
+        <v>28390</v>
       </c>
     </row>
     <row r="104">
@@ -2085,11 +2192,12 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>31629</v>
+        <v>29918</v>
       </c>
       <c r="D104" t="n">
         <v>61075</v>
       </c>
+      <c r="E104" t="inlineStr"/>
     </row>
     <row r="105">
       <c r="A105" t="n">
@@ -2101,9 +2209,10 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>345</v>
-      </c>
-      <c r="D105" t="n">
+        <v>344</v>
+      </c>
+      <c r="D105" t="inlineStr"/>
+      <c r="E105" t="n">
         <v>61075</v>
       </c>
     </row>
@@ -2117,10 +2226,11 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>31629</v>
-      </c>
-      <c r="D106" t="n">
-        <v>31973</v>
+        <v>29918</v>
+      </c>
+      <c r="D106" t="inlineStr"/>
+      <c r="E106" t="n">
+        <v>30259</v>
       </c>
     </row>
     <row r="107">
@@ -2133,11 +2243,12 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>33594</v>
+        <v>32284</v>
       </c>
       <c r="D107" t="n">
         <v>64620</v>
       </c>
+      <c r="E107" t="inlineStr"/>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -2149,9 +2260,10 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>353</v>
-      </c>
-      <c r="D108" t="n">
+        <v>352</v>
+      </c>
+      <c r="D108" t="inlineStr"/>
+      <c r="E108" t="n">
         <v>64620</v>
       </c>
     </row>
@@ -2165,10 +2277,11 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>33594</v>
-      </c>
-      <c r="D109" t="n">
-        <v>33948</v>
+        <v>32284</v>
+      </c>
+      <c r="D109" t="inlineStr"/>
+      <c r="E109" t="n">
+        <v>32639</v>
       </c>
     </row>
     <row r="110">
@@ -2181,11 +2294,12 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>34797</v>
+        <v>32150</v>
       </c>
       <c r="D110" t="n">
         <v>68265</v>
       </c>
+      <c r="E110" t="inlineStr"/>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -2199,7 +2313,8 @@
       <c r="C111" t="n">
         <v>364</v>
       </c>
-      <c r="D111" t="n">
+      <c r="D111" t="inlineStr"/>
+      <c r="E111" t="n">
         <v>68265</v>
       </c>
     </row>
@@ -2213,10 +2328,11 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>34797</v>
-      </c>
-      <c r="D112" t="n">
-        <v>35162</v>
+        <v>32150</v>
+      </c>
+      <c r="D112" t="inlineStr"/>
+      <c r="E112" t="n">
+        <v>32514</v>
       </c>
     </row>
     <row r="113">
@@ -2229,11 +2345,12 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>34486</v>
+        <v>36192</v>
       </c>
       <c r="D113" t="n">
         <v>72010</v>
       </c>
+      <c r="E113" t="inlineStr"/>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -2245,9 +2362,10 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>368</v>
-      </c>
-      <c r="D114" t="n">
+        <v>369</v>
+      </c>
+      <c r="D114" t="inlineStr"/>
+      <c r="E114" t="n">
         <v>72010</v>
       </c>
     </row>
@@ -2261,10 +2379,11 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>34486</v>
-      </c>
-      <c r="D115" t="n">
-        <v>34861</v>
+        <v>36192</v>
+      </c>
+      <c r="D115" t="inlineStr"/>
+      <c r="E115" t="n">
+        <v>36565</v>
       </c>
     </row>
     <row r="116">
@@ -2277,11 +2396,12 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>39616</v>
+        <v>40726</v>
       </c>
       <c r="D116" t="n">
         <v>75855</v>
       </c>
+      <c r="E116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="n">
@@ -2293,9 +2413,10 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>384</v>
-      </c>
-      <c r="D117" t="n">
+        <v>383</v>
+      </c>
+      <c r="D117" t="inlineStr"/>
+      <c r="E117" t="n">
         <v>75855</v>
       </c>
     </row>
@@ -2309,10 +2430,11 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>39616</v>
-      </c>
-      <c r="D118" t="n">
-        <v>39996</v>
+        <v>40726</v>
+      </c>
+      <c r="D118" t="inlineStr"/>
+      <c r="E118" t="n">
+        <v>41111</v>
       </c>
     </row>
     <row r="119">
@@ -2325,11 +2447,12 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>40813</v>
+        <v>42111</v>
       </c>
       <c r="D119" t="n">
         <v>79800</v>
       </c>
+      <c r="E119" t="inlineStr"/>
     </row>
     <row r="120">
       <c r="A120" t="n">
@@ -2343,7 +2466,8 @@
       <c r="C120" t="n">
         <v>392</v>
       </c>
-      <c r="D120" t="n">
+      <c r="D120" t="inlineStr"/>
+      <c r="E120" t="n">
         <v>79800</v>
       </c>
     </row>
@@ -2357,10 +2481,11 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>40813</v>
-      </c>
-      <c r="D121" t="n">
-        <v>41207</v>
+        <v>42111</v>
+      </c>
+      <c r="D121" t="inlineStr"/>
+      <c r="E121" t="n">
+        <v>42505</v>
       </c>
     </row>
     <row r="122">
@@ -2373,11 +2498,12 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>39304</v>
+        <v>41819</v>
       </c>
       <c r="D122" t="n">
         <v>83845</v>
       </c>
+      <c r="E122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" t="n">
@@ -2389,9 +2515,10 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>405</v>
-      </c>
-      <c r="D123" t="n">
+        <v>407</v>
+      </c>
+      <c r="D123" t="inlineStr"/>
+      <c r="E123" t="n">
         <v>83845</v>
       </c>
     </row>
@@ -2405,10 +2532,11 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>39304</v>
-      </c>
-      <c r="D124" t="n">
-        <v>39705</v>
+        <v>41819</v>
+      </c>
+      <c r="D124" t="inlineStr"/>
+      <c r="E124" t="n">
+        <v>42223</v>
       </c>
     </row>
     <row r="125">
@@ -2421,11 +2549,12 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>44920</v>
+        <v>43412</v>
       </c>
       <c r="D125" t="n">
         <v>87990</v>
       </c>
+      <c r="E125" t="inlineStr"/>
     </row>
     <row r="126">
       <c r="A126" t="n">
@@ -2439,7 +2568,8 @@
       <c r="C126" t="n">
         <v>416</v>
       </c>
-      <c r="D126" t="n">
+      <c r="D126" t="inlineStr"/>
+      <c r="E126" t="n">
         <v>87990</v>
       </c>
     </row>
@@ -2453,10 +2583,11 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>44920</v>
-      </c>
-      <c r="D127" t="n">
-        <v>45332</v>
+        <v>43412</v>
+      </c>
+      <c r="D127" t="inlineStr"/>
+      <c r="E127" t="n">
+        <v>43821</v>
       </c>
     </row>
     <row r="128">
@@ -2469,11 +2600,12 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>46711</v>
+        <v>45810</v>
       </c>
       <c r="D128" t="n">
         <v>92235</v>
       </c>
+      <c r="E128" t="inlineStr"/>
     </row>
     <row r="129">
       <c r="A129" t="n">
@@ -2485,9 +2617,10 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>426</v>
-      </c>
-      <c r="D129" t="n">
+        <v>420</v>
+      </c>
+      <c r="D129" t="inlineStr"/>
+      <c r="E129" t="n">
         <v>92235</v>
       </c>
     </row>
@@ -2501,10 +2634,11 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>46711</v>
-      </c>
-      <c r="D130" t="n">
-        <v>47135</v>
+        <v>45810</v>
+      </c>
+      <c r="D130" t="inlineStr"/>
+      <c r="E130" t="n">
+        <v>46232</v>
       </c>
     </row>
     <row r="131">
@@ -2517,11 +2651,12 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>48838</v>
+        <v>47231</v>
       </c>
       <c r="D131" t="n">
         <v>96580</v>
       </c>
+      <c r="E131" t="inlineStr"/>
     </row>
     <row r="132">
       <c r="A132" t="n">
@@ -2533,9 +2668,10 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>431</v>
-      </c>
-      <c r="D132" t="n">
+        <v>433</v>
+      </c>
+      <c r="D132" t="inlineStr"/>
+      <c r="E132" t="n">
         <v>96580</v>
       </c>
     </row>
@@ -2549,10 +2685,11 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>48838</v>
-      </c>
-      <c r="D133" t="n">
-        <v>49275</v>
+        <v>47231</v>
+      </c>
+      <c r="D133" t="inlineStr"/>
+      <c r="E133" t="n">
+        <v>47659</v>
       </c>
     </row>
     <row r="134">
@@ -2565,11 +2702,12 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>51390</v>
+        <v>52572</v>
       </c>
       <c r="D134" t="n">
         <v>101025</v>
       </c>
+      <c r="E134" t="inlineStr"/>
     </row>
     <row r="135">
       <c r="A135" t="n">
@@ -2581,9 +2719,10 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>444</v>
-      </c>
-      <c r="D135" t="n">
+        <v>445</v>
+      </c>
+      <c r="D135" t="inlineStr"/>
+      <c r="E135" t="n">
         <v>101025</v>
       </c>
     </row>
@@ -2597,10 +2736,11 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>51390</v>
-      </c>
-      <c r="D136" t="n">
-        <v>51832</v>
+        <v>52572</v>
+      </c>
+      <c r="D136" t="inlineStr"/>
+      <c r="E136" t="n">
+        <v>53015</v>
       </c>
     </row>
     <row r="137">
@@ -2613,11 +2753,12 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>52047</v>
+        <v>51579</v>
       </c>
       <c r="D137" t="n">
         <v>105570</v>
       </c>
+      <c r="E137" t="inlineStr"/>
     </row>
     <row r="138">
       <c r="A138" t="n">
@@ -2631,7 +2772,8 @@
       <c r="C138" t="n">
         <v>451</v>
       </c>
-      <c r="D138" t="n">
+      <c r="D138" t="inlineStr"/>
+      <c r="E138" t="n">
         <v>105570</v>
       </c>
     </row>
@@ -2645,10 +2787,11 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>52047</v>
-      </c>
-      <c r="D139" t="n">
-        <v>52499</v>
+        <v>51579</v>
+      </c>
+      <c r="D139" t="inlineStr"/>
+      <c r="E139" t="n">
+        <v>52031</v>
       </c>
     </row>
     <row r="140">
@@ -2661,11 +2804,12 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>52474</v>
+        <v>50479</v>
       </c>
       <c r="D140" t="n">
         <v>110215</v>
       </c>
+      <c r="E140" t="inlineStr"/>
     </row>
     <row r="141">
       <c r="A141" t="n">
@@ -2677,9 +2821,10 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>461</v>
-      </c>
-      <c r="D141" t="n">
+        <v>463</v>
+      </c>
+      <c r="D141" t="inlineStr"/>
+      <c r="E141" t="n">
         <v>110215</v>
       </c>
     </row>
@@ -2693,10 +2838,11 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>52474</v>
-      </c>
-      <c r="D142" t="n">
-        <v>52936</v>
+        <v>50479</v>
+      </c>
+      <c r="D142" t="inlineStr"/>
+      <c r="E142" t="n">
+        <v>50941</v>
       </c>
     </row>
     <row r="143">
@@ -2709,11 +2855,12 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>56950</v>
+        <v>55608</v>
       </c>
       <c r="D143" t="n">
         <v>114960</v>
       </c>
+      <c r="E143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -2725,9 +2872,10 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>475</v>
-      </c>
-      <c r="D144" t="n">
+        <v>473</v>
+      </c>
+      <c r="D144" t="inlineStr"/>
+      <c r="E144" t="n">
         <v>114960</v>
       </c>
     </row>
@@ -2741,10 +2889,11 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>56950</v>
-      </c>
-      <c r="D145" t="n">
-        <v>57425</v>
+        <v>55608</v>
+      </c>
+      <c r="D145" t="inlineStr"/>
+      <c r="E145" t="n">
+        <v>56081</v>
       </c>
     </row>
     <row r="146">
@@ -2757,11 +2906,12 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>58644</v>
+        <v>62064</v>
       </c>
       <c r="D146" t="n">
         <v>119805</v>
       </c>
+      <c r="E146" t="inlineStr"/>
     </row>
     <row r="147">
       <c r="A147" t="n">
@@ -2775,7 +2925,8 @@
       <c r="C147" t="n">
         <v>485</v>
       </c>
-      <c r="D147" t="n">
+      <c r="D147" t="inlineStr"/>
+      <c r="E147" t="n">
         <v>119805</v>
       </c>
     </row>
@@ -2789,10 +2940,11 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>58644</v>
-      </c>
-      <c r="D148" t="n">
-        <v>59127</v>
+        <v>62064</v>
+      </c>
+      <c r="D148" t="inlineStr"/>
+      <c r="E148" t="n">
+        <v>62551</v>
       </c>
     </row>
     <row r="149">
@@ -2805,11 +2957,12 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>62203</v>
+        <v>60678</v>
       </c>
       <c r="D149" t="n">
         <v>124750</v>
       </c>
+      <c r="E149" t="inlineStr"/>
     </row>
     <row r="150">
       <c r="A150" t="n">
@@ -2821,9 +2974,10 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>495</v>
-      </c>
-      <c r="D150" t="n">
+        <v>493</v>
+      </c>
+      <c r="D150" t="inlineStr"/>
+      <c r="E150" t="n">
         <v>124750</v>
       </c>
     </row>
@@ -2837,10 +2991,11 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>62203</v>
-      </c>
-      <c r="D151" t="n">
-        <v>62696</v>
+        <v>60678</v>
+      </c>
+      <c r="D151" t="inlineStr"/>
+      <c r="E151" t="n">
+        <v>61171</v>
       </c>
     </row>
     <row r="152">
@@ -2853,11 +3008,12 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>63879</v>
+        <v>58062</v>
       </c>
       <c r="D152" t="n">
         <v>129795</v>
       </c>
+      <c r="E152" t="inlineStr"/>
     </row>
     <row r="153">
       <c r="A153" t="n">
@@ -2869,9 +3025,10 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>504</v>
-      </c>
-      <c r="D153" t="n">
+        <v>502</v>
+      </c>
+      <c r="D153" t="inlineStr"/>
+      <c r="E153" t="n">
         <v>129795</v>
       </c>
     </row>
@@ -2885,10 +3042,11 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>63879</v>
-      </c>
-      <c r="D154" t="n">
-        <v>64383</v>
+        <v>58062</v>
+      </c>
+      <c r="D154" t="inlineStr"/>
+      <c r="E154" t="n">
+        <v>58565</v>
       </c>
     </row>
     <row r="155">
@@ -2901,11 +3059,12 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>68220</v>
+        <v>68810</v>
       </c>
       <c r="D155" t="n">
         <v>134940</v>
       </c>
+      <c r="E155" t="inlineStr"/>
     </row>
     <row r="156">
       <c r="A156" t="n">
@@ -2917,9 +3076,10 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>512</v>
-      </c>
-      <c r="D156" t="n">
+        <v>514</v>
+      </c>
+      <c r="D156" t="inlineStr"/>
+      <c r="E156" t="n">
         <v>134940</v>
       </c>
     </row>
@@ -2933,10 +3093,11 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>68220</v>
-      </c>
-      <c r="D157" t="n">
-        <v>68729</v>
+        <v>68810</v>
+      </c>
+      <c r="D157" t="inlineStr"/>
+      <c r="E157" t="n">
+        <v>69326</v>
       </c>
     </row>
     <row r="158">
@@ -2949,11 +3110,12 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>71213</v>
+        <v>70795</v>
       </c>
       <c r="D158" t="n">
         <v>140185</v>
       </c>
+      <c r="E158" t="inlineStr"/>
     </row>
     <row r="159">
       <c r="A159" t="n">
@@ -2965,9 +3127,10 @@
         </is>
       </c>
       <c r="C159" t="n">
-        <v>524</v>
-      </c>
-      <c r="D159" t="n">
+        <v>520</v>
+      </c>
+      <c r="D159" t="inlineStr"/>
+      <c r="E159" t="n">
         <v>140185</v>
       </c>
     </row>
@@ -2981,10 +3144,11 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>71213</v>
-      </c>
-      <c r="D160" t="n">
-        <v>71737</v>
+        <v>70795</v>
+      </c>
+      <c r="D160" t="inlineStr"/>
+      <c r="E160" t="n">
+        <v>71319</v>
       </c>
     </row>
     <row r="161">
@@ -2997,11 +3161,12 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>75593</v>
+        <v>71414</v>
       </c>
       <c r="D161" t="n">
         <v>145530</v>
       </c>
+      <c r="E161" t="inlineStr"/>
     </row>
     <row r="162">
       <c r="A162" t="n">
@@ -3013,9 +3178,10 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>531</v>
-      </c>
-      <c r="D162" t="n">
+        <v>534</v>
+      </c>
+      <c r="D162" t="inlineStr"/>
+      <c r="E162" t="n">
         <v>145530</v>
       </c>
     </row>
@@ -3029,10 +3195,11 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>75593</v>
-      </c>
-      <c r="D163" t="n">
-        <v>76123</v>
+        <v>71414</v>
+      </c>
+      <c r="D163" t="inlineStr"/>
+      <c r="E163" t="n">
+        <v>71946</v>
       </c>
     </row>
     <row r="164">
@@ -3045,11 +3212,12 @@
         </is>
       </c>
       <c r="C164" t="n">
-        <v>79021</v>
+        <v>76617</v>
       </c>
       <c r="D164" t="n">
         <v>150975</v>
       </c>
+      <c r="E164" t="inlineStr"/>
     </row>
     <row r="165">
       <c r="A165" t="n">
@@ -3061,9 +3229,10 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>542</v>
-      </c>
-      <c r="D165" t="n">
+        <v>544</v>
+      </c>
+      <c r="D165" t="inlineStr"/>
+      <c r="E165" t="n">
         <v>150975</v>
       </c>
     </row>
@@ -3077,10 +3246,11 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>79021</v>
-      </c>
-      <c r="D166" t="n">
-        <v>79563</v>
+        <v>76617</v>
+      </c>
+      <c r="D166" t="inlineStr"/>
+      <c r="E166" t="n">
+        <v>77163</v>
       </c>
     </row>
     <row r="167">
@@ -3093,11 +3263,12 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>78873</v>
+        <v>80531</v>
       </c>
       <c r="D167" t="n">
         <v>156520</v>
       </c>
+      <c r="E167" t="inlineStr"/>
     </row>
     <row r="168">
       <c r="A168" t="n">
@@ -3109,9 +3280,10 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>548</v>
-      </c>
-      <c r="D168" t="n">
+        <v>551</v>
+      </c>
+      <c r="D168" t="inlineStr"/>
+      <c r="E168" t="n">
         <v>156520</v>
       </c>
     </row>
@@ -3125,10 +3297,11 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>78873</v>
-      </c>
-      <c r="D169" t="n">
-        <v>79427</v>
+        <v>80531</v>
+      </c>
+      <c r="D169" t="inlineStr"/>
+      <c r="E169" t="n">
+        <v>81082</v>
       </c>
     </row>
     <row r="170">
@@ -3141,11 +3314,12 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>86662</v>
+        <v>80259</v>
       </c>
       <c r="D170" t="n">
         <v>162165</v>
       </c>
+      <c r="E170" t="inlineStr"/>
     </row>
     <row r="171">
       <c r="A171" t="n">
@@ -3157,9 +3331,10 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>566</v>
-      </c>
-      <c r="D171" t="n">
+        <v>565</v>
+      </c>
+      <c r="D171" t="inlineStr"/>
+      <c r="E171" t="n">
         <v>162165</v>
       </c>
     </row>
@@ -3173,10 +3348,11 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>86662</v>
-      </c>
-      <c r="D172" t="n">
-        <v>87224</v>
+        <v>80259</v>
+      </c>
+      <c r="D172" t="inlineStr"/>
+      <c r="E172" t="n">
+        <v>80823</v>
       </c>
     </row>
     <row r="173">
@@ -3189,11 +3365,12 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>83937</v>
+        <v>84567</v>
       </c>
       <c r="D173" t="n">
         <v>167910</v>
       </c>
+      <c r="E173" t="inlineStr"/>
     </row>
     <row r="174">
       <c r="A174" t="n">
@@ -3205,9 +3382,10 @@
         </is>
       </c>
       <c r="C174" t="n">
-        <v>572</v>
-      </c>
-      <c r="D174" t="n">
+        <v>575</v>
+      </c>
+      <c r="D174" t="inlineStr"/>
+      <c r="E174" t="n">
         <v>167910</v>
       </c>
     </row>
@@ -3221,10 +3399,11 @@
         </is>
       </c>
       <c r="C175" t="n">
-        <v>83937</v>
-      </c>
-      <c r="D175" t="n">
-        <v>84512</v>
+        <v>84567</v>
+      </c>
+      <c r="D175" t="inlineStr"/>
+      <c r="E175" t="n">
+        <v>85143</v>
       </c>
     </row>
     <row r="176">
@@ -3237,11 +3416,12 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>83180</v>
+        <v>87191</v>
       </c>
       <c r="D176" t="n">
         <v>173755</v>
       </c>
+      <c r="E176" t="inlineStr"/>
     </row>
     <row r="177">
       <c r="A177" t="n">
@@ -3255,7 +3435,8 @@
       <c r="C177" t="n">
         <v>584</v>
       </c>
-      <c r="D177" t="n">
+      <c r="D177" t="inlineStr"/>
+      <c r="E177" t="n">
         <v>173755</v>
       </c>
     </row>
@@ -3269,10 +3450,11 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>83180</v>
-      </c>
-      <c r="D178" t="n">
-        <v>83761</v>
+        <v>87191</v>
+      </c>
+      <c r="D178" t="inlineStr"/>
+      <c r="E178" t="n">
+        <v>87777</v>
       </c>
     </row>
     <row r="179">
@@ -3285,11 +3467,12 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>85534</v>
+        <v>86712</v>
       </c>
       <c r="D179" t="n">
         <v>179700</v>
       </c>
+      <c r="E179" t="inlineStr"/>
     </row>
     <row r="180">
       <c r="A180" t="n">
@@ -3301,9 +3484,10 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>593</v>
-      </c>
-      <c r="D180" t="n">
+        <v>592</v>
+      </c>
+      <c r="D180" t="inlineStr"/>
+      <c r="E180" t="n">
         <v>179700</v>
       </c>
     </row>
@@ -3317,10 +3501,11 @@
         </is>
       </c>
       <c r="C181" t="n">
-        <v>85534</v>
-      </c>
-      <c r="D181" t="n">
-        <v>86125</v>
+        <v>86712</v>
+      </c>
+      <c r="D181" t="inlineStr"/>
+      <c r="E181" t="n">
+        <v>87306</v>
       </c>
     </row>
     <row r="182">
@@ -3333,11 +3518,12 @@
         </is>
       </c>
       <c r="C182" t="n">
-        <v>94896</v>
+        <v>91370</v>
       </c>
       <c r="D182" t="n">
         <v>185745</v>
       </c>
+      <c r="E182" t="inlineStr"/>
     </row>
     <row r="183">
       <c r="A183" t="n">
@@ -3349,9 +3535,10 @@
         </is>
       </c>
       <c r="C183" t="n">
-        <v>606</v>
-      </c>
-      <c r="D183" t="n">
+        <v>605</v>
+      </c>
+      <c r="D183" t="inlineStr"/>
+      <c r="E183" t="n">
         <v>185745</v>
       </c>
     </row>
@@ -3365,10 +3552,11 @@
         </is>
       </c>
       <c r="C184" t="n">
-        <v>94896</v>
-      </c>
-      <c r="D184" t="n">
-        <v>95497</v>
+        <v>91370</v>
+      </c>
+      <c r="D184" t="inlineStr"/>
+      <c r="E184" t="n">
+        <v>91975</v>
       </c>
     </row>
     <row r="185">
@@ -3381,11 +3569,12 @@
         </is>
       </c>
       <c r="C185" t="n">
-        <v>91613</v>
+        <v>99888</v>
       </c>
       <c r="D185" t="n">
         <v>191890</v>
       </c>
+      <c r="E185" t="inlineStr"/>
     </row>
     <row r="186">
       <c r="A186" t="n">
@@ -3397,9 +3586,10 @@
         </is>
       </c>
       <c r="C186" t="n">
-        <v>616</v>
-      </c>
-      <c r="D186" t="n">
+        <v>615</v>
+      </c>
+      <c r="D186" t="inlineStr"/>
+      <c r="E186" t="n">
         <v>191890</v>
       </c>
     </row>
@@ -3413,10 +3603,11 @@
         </is>
       </c>
       <c r="C187" t="n">
-        <v>91613</v>
-      </c>
-      <c r="D187" t="n">
-        <v>92229</v>
+        <v>99888</v>
+      </c>
+      <c r="D187" t="inlineStr"/>
+      <c r="E187" t="n">
+        <v>100498</v>
       </c>
     </row>
     <row r="188">
@@ -3429,11 +3620,12 @@
         </is>
       </c>
       <c r="C188" t="n">
-        <v>96212</v>
+        <v>97997</v>
       </c>
       <c r="D188" t="n">
         <v>198135</v>
       </c>
+      <c r="E188" t="inlineStr"/>
     </row>
     <row r="189">
       <c r="A189" t="n">
@@ -3445,9 +3637,10 @@
         </is>
       </c>
       <c r="C189" t="n">
-        <v>623</v>
-      </c>
-      <c r="D189" t="n">
+        <v>625</v>
+      </c>
+      <c r="D189" t="inlineStr"/>
+      <c r="E189" t="n">
         <v>198135</v>
       </c>
     </row>
@@ -3461,10 +3654,11 @@
         </is>
       </c>
       <c r="C190" t="n">
-        <v>96212</v>
-      </c>
-      <c r="D190" t="n">
-        <v>96835</v>
+        <v>97997</v>
+      </c>
+      <c r="D190" t="inlineStr"/>
+      <c r="E190" t="n">
+        <v>98622</v>
       </c>
     </row>
     <row r="191">
@@ -3477,11 +3671,12 @@
         </is>
       </c>
       <c r="C191" t="n">
-        <v>98584</v>
+        <v>104668</v>
       </c>
       <c r="D191" t="n">
         <v>204480</v>
       </c>
+      <c r="E191" t="inlineStr"/>
     </row>
     <row r="192">
       <c r="A192" t="n">
@@ -3493,9 +3688,10 @@
         </is>
       </c>
       <c r="C192" t="n">
-        <v>632</v>
-      </c>
-      <c r="D192" t="n">
+        <v>634</v>
+      </c>
+      <c r="D192" t="inlineStr"/>
+      <c r="E192" t="n">
         <v>204480</v>
       </c>
     </row>
@@ -3509,10 +3705,11 @@
         </is>
       </c>
       <c r="C193" t="n">
-        <v>98584</v>
-      </c>
-      <c r="D193" t="n">
-        <v>99218</v>
+        <v>104668</v>
+      </c>
+      <c r="D193" t="inlineStr"/>
+      <c r="E193" t="n">
+        <v>105299</v>
       </c>
     </row>
     <row r="194">
@@ -3525,11 +3722,12 @@
         </is>
       </c>
       <c r="C194" t="n">
-        <v>100733</v>
+        <v>98354</v>
       </c>
       <c r="D194" t="n">
         <v>210925</v>
       </c>
+      <c r="E194" t="inlineStr"/>
     </row>
     <row r="195">
       <c r="A195" t="n">
@@ -3543,7 +3741,8 @@
       <c r="C195" t="n">
         <v>640</v>
       </c>
-      <c r="D195" t="n">
+      <c r="D195" t="inlineStr"/>
+      <c r="E195" t="n">
         <v>210925</v>
       </c>
     </row>
@@ -3557,10 +3756,11 @@
         </is>
       </c>
       <c r="C196" t="n">
-        <v>100733</v>
-      </c>
-      <c r="D196" t="n">
-        <v>101379</v>
+        <v>98354</v>
+      </c>
+      <c r="D196" t="inlineStr"/>
+      <c r="E196" t="n">
+        <v>98997</v>
       </c>
     </row>
     <row r="197">
@@ -3573,11 +3773,12 @@
         </is>
       </c>
       <c r="C197" t="n">
-        <v>109172</v>
+        <v>109545</v>
       </c>
       <c r="D197" t="n">
         <v>217470</v>
       </c>
+      <c r="E197" t="inlineStr"/>
     </row>
     <row r="198">
       <c r="A198" t="n">
@@ -3589,9 +3790,10 @@
         </is>
       </c>
       <c r="C198" t="n">
-        <v>655</v>
-      </c>
-      <c r="D198" t="n">
+        <v>652</v>
+      </c>
+      <c r="D198" t="inlineStr"/>
+      <c r="E198" t="n">
         <v>217470</v>
       </c>
     </row>
@@ -3605,10 +3807,11 @@
         </is>
       </c>
       <c r="C199" t="n">
-        <v>109172</v>
-      </c>
-      <c r="D199" t="n">
-        <v>109830</v>
+        <v>109545</v>
+      </c>
+      <c r="D199" t="inlineStr"/>
+      <c r="E199" t="n">
+        <v>110195</v>
       </c>
     </row>
     <row r="200">
@@ -3621,11 +3824,12 @@
         </is>
       </c>
       <c r="C200" t="n">
-        <v>113479</v>
+        <v>109801</v>
       </c>
       <c r="D200" t="n">
         <v>224115</v>
       </c>
+      <c r="E200" t="inlineStr"/>
     </row>
     <row r="201">
       <c r="A201" t="n">
@@ -3637,9 +3841,10 @@
         </is>
       </c>
       <c r="C201" t="n">
-        <v>660</v>
-      </c>
-      <c r="D201" t="n">
+        <v>666</v>
+      </c>
+      <c r="D201" t="inlineStr"/>
+      <c r="E201" t="n">
         <v>224115</v>
       </c>
     </row>
@@ -3653,10 +3858,11 @@
         </is>
       </c>
       <c r="C202" t="n">
-        <v>113479</v>
-      </c>
-      <c r="D202" t="n">
-        <v>114138</v>
+        <v>109801</v>
+      </c>
+      <c r="D202" t="inlineStr"/>
+      <c r="E202" t="n">
+        <v>110463</v>
       </c>
     </row>
     <row r="203">
@@ -3669,11 +3875,12 @@
         </is>
       </c>
       <c r="C203" t="n">
-        <v>120288</v>
+        <v>111998</v>
       </c>
       <c r="D203" t="n">
         <v>230860</v>
       </c>
+      <c r="E203" t="inlineStr"/>
     </row>
     <row r="204">
       <c r="A204" t="n">
@@ -3685,9 +3892,10 @@
         </is>
       </c>
       <c r="C204" t="n">
-        <v>672</v>
-      </c>
-      <c r="D204" t="n">
+        <v>676</v>
+      </c>
+      <c r="D204" t="inlineStr"/>
+      <c r="E204" t="n">
         <v>230860</v>
       </c>
     </row>
@@ -3701,10 +3909,11 @@
         </is>
       </c>
       <c r="C205" t="n">
-        <v>120288</v>
-      </c>
-      <c r="D205" t="n">
-        <v>120962</v>
+        <v>111998</v>
+      </c>
+      <c r="D205" t="inlineStr"/>
+      <c r="E205" t="n">
+        <v>112668</v>
       </c>
     </row>
     <row r="206">
@@ -3717,11 +3926,12 @@
         </is>
       </c>
       <c r="C206" t="n">
-        <v>118553</v>
+        <v>115466</v>
       </c>
       <c r="D206" t="n">
         <v>237705</v>
       </c>
+      <c r="E206" t="inlineStr"/>
     </row>
     <row r="207">
       <c r="A207" t="n">
@@ -3733,9 +3943,10 @@
         </is>
       </c>
       <c r="C207" t="n">
-        <v>686</v>
-      </c>
-      <c r="D207" t="n">
+        <v>685</v>
+      </c>
+      <c r="D207" t="inlineStr"/>
+      <c r="E207" t="n">
         <v>237705</v>
       </c>
     </row>
@@ -3749,10 +3960,11 @@
         </is>
       </c>
       <c r="C208" t="n">
-        <v>118553</v>
-      </c>
-      <c r="D208" t="n">
-        <v>119238</v>
+        <v>115466</v>
+      </c>
+      <c r="D208" t="inlineStr"/>
+      <c r="E208" t="n">
+        <v>116148</v>
       </c>
     </row>
     <row r="209">
@@ -3765,11 +3977,12 @@
         </is>
       </c>
       <c r="C209" t="n">
-        <v>125937</v>
+        <v>119527</v>
       </c>
       <c r="D209" t="n">
         <v>244650</v>
       </c>
+      <c r="E209" t="inlineStr"/>
     </row>
     <row r="210">
       <c r="A210" t="n">
@@ -3781,9 +3994,10 @@
         </is>
       </c>
       <c r="C210" t="n">
-        <v>691</v>
-      </c>
-      <c r="D210" t="n">
+        <v>693</v>
+      </c>
+      <c r="D210" t="inlineStr"/>
+      <c r="E210" t="n">
         <v>244650</v>
       </c>
     </row>
@@ -3797,10 +4011,11 @@
         </is>
       </c>
       <c r="C211" t="n">
-        <v>125937</v>
-      </c>
-      <c r="D211" t="n">
-        <v>126634</v>
+        <v>119527</v>
+      </c>
+      <c r="D211" t="inlineStr"/>
+      <c r="E211" t="n">
+        <v>120220</v>
       </c>
     </row>
     <row r="212">
@@ -3813,11 +4028,12 @@
         </is>
       </c>
       <c r="C212" t="n">
-        <v>119292</v>
+        <v>128785</v>
       </c>
       <c r="D212" t="n">
         <v>251695</v>
       </c>
+      <c r="E212" t="inlineStr"/>
     </row>
     <row r="213">
       <c r="A213" t="n">
@@ -3829,9 +4045,10 @@
         </is>
       </c>
       <c r="C213" t="n">
-        <v>705</v>
-      </c>
-      <c r="D213" t="n">
+        <v>703</v>
+      </c>
+      <c r="D213" t="inlineStr"/>
+      <c r="E213" t="n">
         <v>251695</v>
       </c>
     </row>
@@ -3845,10 +4062,11 @@
         </is>
       </c>
       <c r="C214" t="n">
-        <v>119292</v>
-      </c>
-      <c r="D214" t="n">
-        <v>119995</v>
+        <v>128785</v>
+      </c>
+      <c r="D214" t="inlineStr"/>
+      <c r="E214" t="n">
+        <v>129488</v>
       </c>
     </row>
     <row r="215">
@@ -3861,11 +4079,12 @@
         </is>
       </c>
       <c r="C215" t="n">
-        <v>133604</v>
+        <v>129159</v>
       </c>
       <c r="D215" t="n">
         <v>258840</v>
       </c>
+      <c r="E215" t="inlineStr"/>
     </row>
     <row r="216">
       <c r="A216" t="n">
@@ -3879,7 +4098,8 @@
       <c r="C216" t="n">
         <v>712</v>
       </c>
-      <c r="D216" t="n">
+      <c r="D216" t="inlineStr"/>
+      <c r="E216" t="n">
         <v>258840</v>
       </c>
     </row>
@@ -3893,10 +4113,11 @@
         </is>
       </c>
       <c r="C217" t="n">
-        <v>133604</v>
-      </c>
-      <c r="D217" t="n">
-        <v>134316</v>
+        <v>129159</v>
+      </c>
+      <c r="D217" t="inlineStr"/>
+      <c r="E217" t="n">
+        <v>129872</v>
       </c>
     </row>
     <row r="218">
@@ -3909,11 +4130,12 @@
         </is>
       </c>
       <c r="C218" t="n">
-        <v>126576</v>
+        <v>133192</v>
       </c>
       <c r="D218" t="n">
         <v>266085</v>
       </c>
+      <c r="E218" t="inlineStr"/>
     </row>
     <row r="219">
       <c r="A219" t="n">
@@ -3925,9 +4147,10 @@
         </is>
       </c>
       <c r="C219" t="n">
-        <v>723</v>
-      </c>
-      <c r="D219" t="n">
+        <v>722</v>
+      </c>
+      <c r="D219" t="inlineStr"/>
+      <c r="E219" t="n">
         <v>266085</v>
       </c>
     </row>
@@ -3941,10 +4164,11 @@
         </is>
       </c>
       <c r="C220" t="n">
-        <v>126576</v>
-      </c>
-      <c r="D220" t="n">
-        <v>127298</v>
+        <v>133192</v>
+      </c>
+      <c r="D220" t="inlineStr"/>
+      <c r="E220" t="n">
+        <v>133916</v>
       </c>
     </row>
     <row r="221">
@@ -3957,11 +4181,12 @@
         </is>
       </c>
       <c r="C221" t="n">
-        <v>129935</v>
+        <v>133258</v>
       </c>
       <c r="D221" t="n">
         <v>273430</v>
       </c>
+      <c r="E221" t="inlineStr"/>
     </row>
     <row r="222">
       <c r="A222" t="n">
@@ -3975,7 +4200,8 @@
       <c r="C222" t="n">
         <v>734</v>
       </c>
-      <c r="D222" t="n">
+      <c r="D222" t="inlineStr"/>
+      <c r="E222" t="n">
         <v>273430</v>
       </c>
     </row>
@@ -3989,10 +4215,11 @@
         </is>
       </c>
       <c r="C223" t="n">
-        <v>129935</v>
-      </c>
-      <c r="D223" t="n">
-        <v>130666</v>
+        <v>133258</v>
+      </c>
+      <c r="D223" t="inlineStr"/>
+      <c r="E223" t="n">
+        <v>133996</v>
       </c>
     </row>
     <row r="224">
@@ -4005,11 +4232,12 @@
         </is>
       </c>
       <c r="C224" t="n">
-        <v>144809</v>
+        <v>139488</v>
       </c>
       <c r="D224" t="n">
         <v>280875</v>
       </c>
+      <c r="E224" t="inlineStr"/>
     </row>
     <row r="225">
       <c r="A225" t="n">
@@ -4023,7 +4251,8 @@
       <c r="C225" t="n">
         <v>744</v>
       </c>
-      <c r="D225" t="n">
+      <c r="D225" t="inlineStr"/>
+      <c r="E225" t="n">
         <v>280875</v>
       </c>
     </row>
@@ -4037,10 +4266,11 @@
         </is>
       </c>
       <c r="C226" t="n">
-        <v>144809</v>
-      </c>
-      <c r="D226" t="n">
-        <v>145554</v>
+        <v>139488</v>
+      </c>
+      <c r="D226" t="inlineStr"/>
+      <c r="E226" t="n">
+        <v>140229</v>
       </c>
     </row>
     <row r="227">
@@ -4053,11 +4283,12 @@
         </is>
       </c>
       <c r="C227" t="n">
-        <v>139940</v>
+        <v>145054</v>
       </c>
       <c r="D227" t="n">
         <v>288420</v>
       </c>
+      <c r="E227" t="inlineStr"/>
     </row>
     <row r="228">
       <c r="A228" t="n">
@@ -4069,9 +4300,10 @@
         </is>
       </c>
       <c r="C228" t="n">
-        <v>754</v>
-      </c>
-      <c r="D228" t="n">
+        <v>748</v>
+      </c>
+      <c r="D228" t="inlineStr"/>
+      <c r="E228" t="n">
         <v>288420</v>
       </c>
     </row>
@@ -4085,10 +4317,11 @@
         </is>
       </c>
       <c r="C229" t="n">
-        <v>139940</v>
-      </c>
-      <c r="D229" t="n">
-        <v>140694</v>
+        <v>145054</v>
+      </c>
+      <c r="D229" t="inlineStr"/>
+      <c r="E229" t="n">
+        <v>145808</v>
       </c>
     </row>
     <row r="230">
@@ -4101,11 +4334,12 @@
         </is>
       </c>
       <c r="C230" t="n">
-        <v>150405</v>
+        <v>145687</v>
       </c>
       <c r="D230" t="n">
         <v>296065</v>
       </c>
+      <c r="E230" t="inlineStr"/>
     </row>
     <row r="231">
       <c r="A231" t="n">
@@ -4117,9 +4351,10 @@
         </is>
       </c>
       <c r="C231" t="n">
-        <v>765</v>
-      </c>
-      <c r="D231" t="n">
+        <v>763</v>
+      </c>
+      <c r="D231" t="inlineStr"/>
+      <c r="E231" t="n">
         <v>296065</v>
       </c>
     </row>
@@ -4133,10 +4368,11 @@
         </is>
       </c>
       <c r="C232" t="n">
-        <v>150405</v>
-      </c>
-      <c r="D232" t="n">
-        <v>151166</v>
+        <v>145687</v>
+      </c>
+      <c r="D232" t="inlineStr"/>
+      <c r="E232" t="n">
+        <v>146452</v>
       </c>
     </row>
     <row r="233">
@@ -4149,11 +4385,12 @@
         </is>
       </c>
       <c r="C233" t="n">
-        <v>154678</v>
+        <v>152456</v>
       </c>
       <c r="D233" t="n">
         <v>303810</v>
       </c>
+      <c r="E233" t="inlineStr"/>
     </row>
     <row r="234">
       <c r="A234" t="n">
@@ -4167,7 +4404,8 @@
       <c r="C234" t="n">
         <v>769</v>
       </c>
-      <c r="D234" t="n">
+      <c r="D234" t="inlineStr"/>
+      <c r="E234" t="n">
         <v>303810</v>
       </c>
     </row>
@@ -4181,10 +4419,11 @@
         </is>
       </c>
       <c r="C235" t="n">
-        <v>154678</v>
-      </c>
-      <c r="D235" t="n">
-        <v>155454</v>
+        <v>152456</v>
+      </c>
+      <c r="D235" t="inlineStr"/>
+      <c r="E235" t="n">
+        <v>153229</v>
       </c>
     </row>
     <row r="236">
@@ -4197,11 +4436,12 @@
         </is>
       </c>
       <c r="C236" t="n">
-        <v>156452</v>
+        <v>152514</v>
       </c>
       <c r="D236" t="n">
         <v>311655</v>
       </c>
+      <c r="E236" t="inlineStr"/>
     </row>
     <row r="237">
       <c r="A237" t="n">
@@ -4213,9 +4453,10 @@
         </is>
       </c>
       <c r="C237" t="n">
-        <v>783</v>
-      </c>
-      <c r="D237" t="n">
+        <v>782</v>
+      </c>
+      <c r="D237" t="inlineStr"/>
+      <c r="E237" t="n">
         <v>311655</v>
       </c>
     </row>
@@ -4229,10 +4470,11 @@
         </is>
       </c>
       <c r="C238" t="n">
-        <v>156452</v>
-      </c>
-      <c r="D238" t="n">
-        <v>157233</v>
+        <v>152514</v>
+      </c>
+      <c r="D238" t="inlineStr"/>
+      <c r="E238" t="n">
+        <v>153297</v>
       </c>
     </row>
     <row r="239">
@@ -4245,11 +4487,12 @@
         </is>
       </c>
       <c r="C239" t="n">
-        <v>158418</v>
+        <v>155853</v>
       </c>
       <c r="D239" t="n">
         <v>319600</v>
       </c>
+      <c r="E239" t="inlineStr"/>
     </row>
     <row r="240">
       <c r="A240" t="n">
@@ -4263,7 +4506,8 @@
       <c r="C240" t="n">
         <v>792</v>
       </c>
-      <c r="D240" t="n">
+      <c r="D240" t="inlineStr"/>
+      <c r="E240" t="n">
         <v>319600</v>
       </c>
     </row>
@@ -4277,10 +4521,11 @@
         </is>
       </c>
       <c r="C241" t="n">
-        <v>158418</v>
-      </c>
-      <c r="D241" t="n">
-        <v>159212</v>
+        <v>155853</v>
+      </c>
+      <c r="D241" t="inlineStr"/>
+      <c r="E241" t="n">
+        <v>156646</v>
       </c>
     </row>
     <row r="242">
@@ -4293,11 +4538,12 @@
         </is>
       </c>
       <c r="C242" t="n">
-        <v>168902</v>
+        <v>165012</v>
       </c>
       <c r="D242" t="n">
         <v>327645</v>
       </c>
+      <c r="E242" t="inlineStr"/>
     </row>
     <row r="243">
       <c r="A243" t="n">
@@ -4309,9 +4555,10 @@
         </is>
       </c>
       <c r="C243" t="n">
-        <v>801</v>
-      </c>
-      <c r="D243" t="n">
+        <v>802</v>
+      </c>
+      <c r="D243" t="inlineStr"/>
+      <c r="E243" t="n">
         <v>327645</v>
       </c>
     </row>
@@ -4325,10 +4572,11 @@
         </is>
       </c>
       <c r="C244" t="n">
-        <v>168902</v>
-      </c>
-      <c r="D244" t="n">
-        <v>169706</v>
+        <v>165012</v>
+      </c>
+      <c r="D244" t="inlineStr"/>
+      <c r="E244" t="n">
+        <v>165817</v>
       </c>
     </row>
     <row r="245">
@@ -4341,11 +4589,12 @@
         </is>
       </c>
       <c r="C245" t="n">
-        <v>172279</v>
+        <v>170783</v>
       </c>
       <c r="D245" t="n">
         <v>335790</v>
       </c>
+      <c r="E245" t="inlineStr"/>
     </row>
     <row r="246">
       <c r="A246" t="n">
@@ -4357,9 +4606,10 @@
         </is>
       </c>
       <c r="C246" t="n">
-        <v>815</v>
-      </c>
-      <c r="D246" t="n">
+        <v>809</v>
+      </c>
+      <c r="D246" t="inlineStr"/>
+      <c r="E246" t="n">
         <v>335790</v>
       </c>
     </row>
@@ -4373,10 +4623,11 @@
         </is>
       </c>
       <c r="C247" t="n">
-        <v>172279</v>
-      </c>
-      <c r="D247" t="n">
-        <v>173092</v>
+        <v>170783</v>
+      </c>
+      <c r="D247" t="inlineStr"/>
+      <c r="E247" t="n">
+        <v>171594</v>
       </c>
     </row>
     <row r="248">
@@ -4389,11 +4640,12 @@
         </is>
       </c>
       <c r="C248" t="n">
-        <v>168987</v>
+        <v>172890</v>
       </c>
       <c r="D248" t="n">
         <v>344035</v>
       </c>
+      <c r="E248" t="inlineStr"/>
     </row>
     <row r="249">
       <c r="A249" t="n">
@@ -4405,9 +4657,10 @@
         </is>
       </c>
       <c r="C249" t="n">
-        <v>823</v>
-      </c>
-      <c r="D249" t="n">
+        <v>822</v>
+      </c>
+      <c r="D249" t="inlineStr"/>
+      <c r="E249" t="n">
         <v>344035</v>
       </c>
     </row>
@@ -4421,10 +4674,11 @@
         </is>
       </c>
       <c r="C250" t="n">
-        <v>168987</v>
-      </c>
-      <c r="D250" t="n">
-        <v>169810</v>
+        <v>172890</v>
+      </c>
+      <c r="D250" t="inlineStr"/>
+      <c r="E250" t="n">
+        <v>173704</v>
       </c>
     </row>
     <row r="251">
@@ -4437,11 +4691,12 @@
         </is>
       </c>
       <c r="C251" t="n">
-        <v>181250</v>
+        <v>176746</v>
       </c>
       <c r="D251" t="n">
         <v>352380</v>
       </c>
+      <c r="E251" t="inlineStr"/>
     </row>
     <row r="252">
       <c r="A252" t="n">
@@ -4453,9 +4708,10 @@
         </is>
       </c>
       <c r="C252" t="n">
-        <v>834</v>
-      </c>
-      <c r="D252" t="n">
+        <v>833</v>
+      </c>
+      <c r="D252" t="inlineStr"/>
+      <c r="E252" t="n">
         <v>352380</v>
       </c>
     </row>
@@ -4469,10 +4725,11 @@
         </is>
       </c>
       <c r="C253" t="n">
-        <v>181250</v>
-      </c>
-      <c r="D253" t="n">
-        <v>182079</v>
+        <v>176746</v>
+      </c>
+      <c r="D253" t="inlineStr"/>
+      <c r="E253" t="n">
+        <v>177581</v>
       </c>
     </row>
     <row r="254">
@@ -4485,11 +4742,12 @@
         </is>
       </c>
       <c r="C254" t="n">
-        <v>174688</v>
+        <v>181678</v>
       </c>
       <c r="D254" t="n">
         <v>360825</v>
       </c>
+      <c r="E254" t="inlineStr"/>
     </row>
     <row r="255">
       <c r="A255" t="n">
@@ -4501,9 +4759,10 @@
         </is>
       </c>
       <c r="C255" t="n">
-        <v>843</v>
-      </c>
-      <c r="D255" t="n">
+        <v>842</v>
+      </c>
+      <c r="D255" t="inlineStr"/>
+      <c r="E255" t="n">
         <v>360825</v>
       </c>
     </row>
@@ -4517,10 +4776,11 @@
         </is>
       </c>
       <c r="C256" t="n">
-        <v>174688</v>
-      </c>
-      <c r="D256" t="n">
-        <v>175528</v>
+        <v>181678</v>
+      </c>
+      <c r="D256" t="inlineStr"/>
+      <c r="E256" t="n">
+        <v>182521</v>
       </c>
     </row>
     <row r="257">
@@ -4533,11 +4793,12 @@
         </is>
       </c>
       <c r="C257" t="n">
-        <v>179295</v>
+        <v>185831</v>
       </c>
       <c r="D257" t="n">
         <v>369370</v>
       </c>
+      <c r="E257" t="inlineStr"/>
     </row>
     <row r="258">
       <c r="A258" t="n">
@@ -4549,9 +4810,10 @@
         </is>
       </c>
       <c r="C258" t="n">
-        <v>853</v>
-      </c>
-      <c r="D258" t="n">
+        <v>855</v>
+      </c>
+      <c r="D258" t="inlineStr"/>
+      <c r="E258" t="n">
         <v>369370</v>
       </c>
     </row>
@@ -4565,10 +4827,11 @@
         </is>
       </c>
       <c r="C259" t="n">
-        <v>179295</v>
-      </c>
-      <c r="D259" t="n">
-        <v>180148</v>
+        <v>185831</v>
+      </c>
+      <c r="D259" t="inlineStr"/>
+      <c r="E259" t="n">
+        <v>186685</v>
       </c>
     </row>
     <row r="260">
@@ -4581,11 +4844,12 @@
         </is>
       </c>
       <c r="C260" t="n">
-        <v>184050</v>
+        <v>191905</v>
       </c>
       <c r="D260" t="n">
         <v>378015</v>
       </c>
+      <c r="E260" t="inlineStr"/>
     </row>
     <row r="261">
       <c r="A261" t="n">
@@ -4597,9 +4861,10 @@
         </is>
       </c>
       <c r="C261" t="n">
-        <v>863</v>
-      </c>
-      <c r="D261" t="n">
+        <v>867</v>
+      </c>
+      <c r="D261" t="inlineStr"/>
+      <c r="E261" t="n">
         <v>378015</v>
       </c>
     </row>
@@ -4613,10 +4878,11 @@
         </is>
       </c>
       <c r="C262" t="n">
-        <v>184050</v>
-      </c>
-      <c r="D262" t="n">
-        <v>184912</v>
+        <v>191905</v>
+      </c>
+      <c r="D262" t="inlineStr"/>
+      <c r="E262" t="n">
+        <v>192767</v>
       </c>
     </row>
     <row r="263">
@@ -4629,11 +4895,12 @@
         </is>
       </c>
       <c r="C263" t="n">
-        <v>199327</v>
+        <v>186676</v>
       </c>
       <c r="D263" t="n">
         <v>386760</v>
       </c>
+      <c r="E263" t="inlineStr"/>
     </row>
     <row r="264">
       <c r="A264" t="n">
@@ -4645,9 +4912,10 @@
         </is>
       </c>
       <c r="C264" t="n">
-        <v>867</v>
-      </c>
-      <c r="D264" t="n">
+        <v>871</v>
+      </c>
+      <c r="D264" t="inlineStr"/>
+      <c r="E264" t="n">
         <v>386760</v>
       </c>
     </row>
@@ -4661,10 +4929,11 @@
         </is>
       </c>
       <c r="C265" t="n">
-        <v>199327</v>
-      </c>
-      <c r="D265" t="n">
-        <v>200197</v>
+        <v>186676</v>
+      </c>
+      <c r="D265" t="inlineStr"/>
+      <c r="E265" t="n">
+        <v>187545</v>
       </c>
     </row>
     <row r="266">
@@ -4677,11 +4946,12 @@
         </is>
       </c>
       <c r="C266" t="n">
-        <v>202718</v>
+        <v>199443</v>
       </c>
       <c r="D266" t="n">
         <v>395605</v>
       </c>
+      <c r="E266" t="inlineStr"/>
     </row>
     <row r="267">
       <c r="A267" t="n">
@@ -4693,9 +4963,10 @@
         </is>
       </c>
       <c r="C267" t="n">
-        <v>884</v>
-      </c>
-      <c r="D267" t="n">
+        <v>881</v>
+      </c>
+      <c r="D267" t="inlineStr"/>
+      <c r="E267" t="n">
         <v>395605</v>
       </c>
     </row>
@@ -4709,10 +4980,11 @@
         </is>
       </c>
       <c r="C268" t="n">
-        <v>202718</v>
-      </c>
-      <c r="D268" t="n">
-        <v>203602</v>
+        <v>199443</v>
+      </c>
+      <c r="D268" t="inlineStr"/>
+      <c r="E268" t="n">
+        <v>200326</v>
       </c>
     </row>
     <row r="269">
@@ -4725,11 +4997,12 @@
         </is>
       </c>
       <c r="C269" t="n">
-        <v>200146</v>
+        <v>199730</v>
       </c>
       <c r="D269" t="n">
         <v>404550</v>
       </c>
+      <c r="E269" t="inlineStr"/>
     </row>
     <row r="270">
       <c r="A270" t="n">
@@ -4741,9 +5014,10 @@
         </is>
       </c>
       <c r="C270" t="n">
-        <v>894</v>
-      </c>
-      <c r="D270" t="n">
+        <v>896</v>
+      </c>
+      <c r="D270" t="inlineStr"/>
+      <c r="E270" t="n">
         <v>404550</v>
       </c>
     </row>
@@ -4757,10 +5031,11 @@
         </is>
       </c>
       <c r="C271" t="n">
-        <v>200146</v>
-      </c>
-      <c r="D271" t="n">
-        <v>201041</v>
+        <v>199730</v>
+      </c>
+      <c r="D271" t="inlineStr"/>
+      <c r="E271" t="n">
+        <v>200622</v>
       </c>
     </row>
     <row r="272">
@@ -4773,11 +5048,12 @@
         </is>
       </c>
       <c r="C272" t="n">
-        <v>205649</v>
+        <v>208025</v>
       </c>
       <c r="D272" t="n">
         <v>413595</v>
       </c>
+      <c r="E272" t="inlineStr"/>
     </row>
     <row r="273">
       <c r="A273" t="n">
@@ -4789,9 +5065,10 @@
         </is>
       </c>
       <c r="C273" t="n">
-        <v>903</v>
-      </c>
-      <c r="D273" t="n">
+        <v>896</v>
+      </c>
+      <c r="D273" t="inlineStr"/>
+      <c r="E273" t="n">
         <v>413595</v>
       </c>
     </row>
@@ -4805,10 +5082,11 @@
         </is>
       </c>
       <c r="C274" t="n">
-        <v>205649</v>
-      </c>
-      <c r="D274" t="n">
-        <v>206555</v>
+        <v>208025</v>
+      </c>
+      <c r="D274" t="inlineStr"/>
+      <c r="E274" t="n">
+        <v>208931</v>
       </c>
     </row>
     <row r="275">
@@ -4821,11 +5099,12 @@
         </is>
       </c>
       <c r="C275" t="n">
-        <v>208775</v>
+        <v>202446</v>
       </c>
       <c r="D275" t="n">
         <v>422740</v>
       </c>
+      <c r="E275" t="inlineStr"/>
     </row>
     <row r="276">
       <c r="A276" t="n">
@@ -4837,9 +5116,10 @@
         </is>
       </c>
       <c r="C276" t="n">
-        <v>913</v>
-      </c>
-      <c r="D276" t="n">
+        <v>911</v>
+      </c>
+      <c r="D276" t="inlineStr"/>
+      <c r="E276" t="n">
         <v>422740</v>
       </c>
     </row>
@@ -4853,10 +5133,11 @@
         </is>
       </c>
       <c r="C277" t="n">
-        <v>208775</v>
-      </c>
-      <c r="D277" t="n">
-        <v>209687</v>
+        <v>202446</v>
+      </c>
+      <c r="D277" t="inlineStr"/>
+      <c r="E277" t="n">
+        <v>203360</v>
       </c>
     </row>
     <row r="278">
@@ -4869,11 +5150,12 @@
         </is>
       </c>
       <c r="C278" t="n">
-        <v>208481</v>
+        <v>222588</v>
       </c>
       <c r="D278" t="n">
         <v>431985</v>
       </c>
+      <c r="E278" t="inlineStr"/>
     </row>
     <row r="279">
       <c r="A279" t="n">
@@ -4885,9 +5167,10 @@
         </is>
       </c>
       <c r="C279" t="n">
-        <v>921</v>
-      </c>
-      <c r="D279" t="n">
+        <v>919</v>
+      </c>
+      <c r="D279" t="inlineStr"/>
+      <c r="E279" t="n">
         <v>431985</v>
       </c>
     </row>
@@ -4901,10 +5184,11 @@
         </is>
       </c>
       <c r="C280" t="n">
-        <v>208481</v>
-      </c>
-      <c r="D280" t="n">
-        <v>209401</v>
+        <v>222588</v>
+      </c>
+      <c r="D280" t="inlineStr"/>
+      <c r="E280" t="n">
+        <v>223512</v>
       </c>
     </row>
     <row r="281">
@@ -4917,11 +5201,12 @@
         </is>
       </c>
       <c r="C281" t="n">
-        <v>218364</v>
+        <v>225562</v>
       </c>
       <c r="D281" t="n">
         <v>441330</v>
       </c>
+      <c r="E281" t="inlineStr"/>
     </row>
     <row r="282">
       <c r="A282" t="n">
@@ -4935,7 +5220,8 @@
       <c r="C282" t="n">
         <v>929</v>
       </c>
-      <c r="D282" t="n">
+      <c r="D282" t="inlineStr"/>
+      <c r="E282" t="n">
         <v>441330</v>
       </c>
     </row>
@@ -4949,10 +5235,11 @@
         </is>
       </c>
       <c r="C283" t="n">
-        <v>218364</v>
-      </c>
-      <c r="D283" t="n">
-        <v>219299</v>
+        <v>225562</v>
+      </c>
+      <c r="D283" t="inlineStr"/>
+      <c r="E283" t="n">
+        <v>226495</v>
       </c>
     </row>
     <row r="284">
@@ -4965,11 +5252,12 @@
         </is>
       </c>
       <c r="C284" t="n">
-        <v>228963</v>
+        <v>221368</v>
       </c>
       <c r="D284" t="n">
         <v>450775</v>
       </c>
+      <c r="E284" t="inlineStr"/>
     </row>
     <row r="285">
       <c r="A285" t="n">
@@ -4981,9 +5269,10 @@
         </is>
       </c>
       <c r="C285" t="n">
-        <v>947</v>
-      </c>
-      <c r="D285" t="n">
+        <v>943</v>
+      </c>
+      <c r="D285" t="inlineStr"/>
+      <c r="E285" t="n">
         <v>450775</v>
       </c>
     </row>
@@ -4997,10 +5286,11 @@
         </is>
       </c>
       <c r="C286" t="n">
-        <v>228963</v>
-      </c>
-      <c r="D286" t="n">
-        <v>229906</v>
+        <v>221368</v>
+      </c>
+      <c r="D286" t="inlineStr"/>
+      <c r="E286" t="n">
+        <v>222309</v>
       </c>
     </row>
     <row r="287">
@@ -5013,11 +5303,12 @@
         </is>
       </c>
       <c r="C287" t="n">
-        <v>230827</v>
+        <v>222860</v>
       </c>
       <c r="D287" t="n">
         <v>460320</v>
       </c>
+      <c r="E287" t="inlineStr"/>
     </row>
     <row r="288">
       <c r="A288" t="n">
@@ -5029,9 +5320,10 @@
         </is>
       </c>
       <c r="C288" t="n">
-        <v>949</v>
-      </c>
-      <c r="D288" t="n">
+        <v>955</v>
+      </c>
+      <c r="D288" t="inlineStr"/>
+      <c r="E288" t="n">
         <v>460320</v>
       </c>
     </row>
@@ -5045,10 +5337,11 @@
         </is>
       </c>
       <c r="C289" t="n">
-        <v>230827</v>
-      </c>
-      <c r="D289" t="n">
-        <v>231779</v>
+        <v>222860</v>
+      </c>
+      <c r="D289" t="inlineStr"/>
+      <c r="E289" t="n">
+        <v>223812</v>
       </c>
     </row>
     <row r="290">
@@ -5061,11 +5354,12 @@
         </is>
       </c>
       <c r="C290" t="n">
-        <v>242907</v>
+        <v>231689</v>
       </c>
       <c r="D290" t="n">
         <v>469965</v>
       </c>
+      <c r="E290" t="inlineStr"/>
     </row>
     <row r="291">
       <c r="A291" t="n">
@@ -5077,9 +5371,10 @@
         </is>
       </c>
       <c r="C291" t="n">
-        <v>957</v>
-      </c>
-      <c r="D291" t="n">
+        <v>964</v>
+      </c>
+      <c r="D291" t="inlineStr"/>
+      <c r="E291" t="n">
         <v>469965</v>
       </c>
     </row>
@@ -5093,10 +5388,11 @@
         </is>
       </c>
       <c r="C292" t="n">
-        <v>242907</v>
-      </c>
-      <c r="D292" t="n">
-        <v>243873</v>
+        <v>231689</v>
+      </c>
+      <c r="D292" t="inlineStr"/>
+      <c r="E292" t="n">
+        <v>232654</v>
       </c>
     </row>
     <row r="293">
@@ -5109,11 +5405,12 @@
         </is>
       </c>
       <c r="C293" t="n">
-        <v>238193</v>
+        <v>236047</v>
       </c>
       <c r="D293" t="n">
         <v>479710</v>
       </c>
+      <c r="E293" t="inlineStr"/>
     </row>
     <row r="294">
       <c r="A294" t="n">
@@ -5125,9 +5422,10 @@
         </is>
       </c>
       <c r="C294" t="n">
-        <v>973</v>
-      </c>
-      <c r="D294" t="n">
+        <v>971</v>
+      </c>
+      <c r="D294" t="inlineStr"/>
+      <c r="E294" t="n">
         <v>479710</v>
       </c>
     </row>
@@ -5141,10 +5439,11 @@
         </is>
       </c>
       <c r="C295" t="n">
-        <v>238193</v>
-      </c>
-      <c r="D295" t="n">
-        <v>239164</v>
+        <v>236047</v>
+      </c>
+      <c r="D295" t="inlineStr"/>
+      <c r="E295" t="n">
+        <v>237018</v>
       </c>
     </row>
     <row r="296">
@@ -5157,11 +5456,12 @@
         </is>
       </c>
       <c r="C296" t="n">
-        <v>244984</v>
+        <v>239352</v>
       </c>
       <c r="D296" t="n">
         <v>489555</v>
       </c>
+      <c r="E296" t="inlineStr"/>
     </row>
     <row r="297">
       <c r="A297" t="n">
@@ -5173,9 +5473,10 @@
         </is>
       </c>
       <c r="C297" t="n">
-        <v>979</v>
-      </c>
-      <c r="D297" t="n">
+        <v>985</v>
+      </c>
+      <c r="D297" t="inlineStr"/>
+      <c r="E297" t="n">
         <v>489555</v>
       </c>
     </row>
@@ -5189,10 +5490,11 @@
         </is>
       </c>
       <c r="C298" t="n">
-        <v>244984</v>
-      </c>
-      <c r="D298" t="n">
-        <v>245966</v>
+        <v>239352</v>
+      </c>
+      <c r="D298" t="inlineStr"/>
+      <c r="E298" t="n">
+        <v>240332</v>
       </c>
     </row>
     <row r="299">
@@ -5205,11 +5507,12 @@
         </is>
       </c>
       <c r="C299" t="n">
-        <v>247242</v>
+        <v>255916</v>
       </c>
       <c r="D299" t="n">
         <v>499500</v>
       </c>
+      <c r="E299" t="inlineStr"/>
     </row>
     <row r="300">
       <c r="A300" t="n">
@@ -5221,9 +5524,10 @@
         </is>
       </c>
       <c r="C300" t="n">
-        <v>990</v>
-      </c>
-      <c r="D300" t="n">
+        <v>994</v>
+      </c>
+      <c r="D300" t="inlineStr"/>
+      <c r="E300" t="n">
         <v>499500</v>
       </c>
     </row>
@@ -5237,10 +5541,11 @@
         </is>
       </c>
       <c r="C301" t="n">
-        <v>247242</v>
-      </c>
-      <c r="D301" t="n">
-        <v>248233</v>
+        <v>255916</v>
+      </c>
+      <c r="D301" t="inlineStr"/>
+      <c r="E301" t="n">
+        <v>256908</v>
       </c>
     </row>
   </sheetData>

</xml_diff>